<commit_message>
Update fuels/PoFDCtAE to cause increases in fuel exports in response to decreases in domestic consumption
</commit_message>
<xml_diff>
--- a/InputData/fuels/PoFDCtAE/Perc of Fuel Demand Changes that Affect Exports.xlsx
+++ b/InputData/fuels/PoFDCtAE/Perc of Fuel Demand Changes that Affect Exports.xlsx
@@ -1,26 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeff-nonadmin\Dropbox (Energy InNovation)\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{190E0567-D228-475F-AE92-CB99F12E58B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28185" windowHeight="12510"/>
+    <workbookView xWindow="2055" yWindow="1065" windowWidth="23535" windowHeight="16185" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
-    <sheet name="PoFDCtAE" sheetId="2" r:id="rId2"/>
+    <sheet name="Data from BFPIaE" sheetId="3" r:id="rId2"/>
+    <sheet name="PoFDCtAE" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="100">
   <si>
     <t>PoFDCtAE Percentage of Fuel Demand Change that Alters Exports</t>
   </si>
@@ -91,9 +106,6 @@
     <t>This variable allows you to specify this behavior for a given country.</t>
   </si>
   <si>
-    <t>a great deal of capacity to increase or decrease its own production</t>
-  </si>
-  <si>
     <t>Saudi Arabia is a major crude oil exporter.  Saudi Arabia's cost to produce</t>
   </si>
   <si>
@@ -121,33 +133,6 @@
     <t>rather than changes in production or imports.</t>
   </si>
   <si>
-    <t>Example 1: The United States</t>
-  </si>
-  <si>
-    <t>Example 2: Saudi Arabia</t>
-  </si>
-  <si>
-    <t>The following examples may help you set this variable wisely:</t>
-  </si>
-  <si>
-    <t>The United States is a major exporter of oil.  The U.S. has</t>
-  </si>
-  <si>
-    <t>to meet demand.  Its oil is not exceptionally cheap to produce and</t>
-  </si>
-  <si>
-    <t>comes in around the global marginal price, accounting for shipping costs.</t>
-  </si>
-  <si>
-    <t>If the U.S. could export more oil profitably, it would already be doing so.</t>
-  </si>
-  <si>
-    <t>Changes in domestic oil demand are likely to be met with changes</t>
-  </si>
-  <si>
-    <t>in production and imports.</t>
-  </si>
-  <si>
     <t>electricity (not used in this variable)</t>
   </si>
   <si>
@@ -262,25 +247,103 @@
     <t>Percentage Change in Demand that Alters Exports (dimensionless) - From type (below)  / To type (right)</t>
   </si>
   <si>
+    <t>Converted to BTU</t>
+  </si>
+  <si>
+    <t>Fuel</t>
+  </si>
+  <si>
+    <t>Production</t>
+  </si>
+  <si>
+    <t>Imports</t>
+  </si>
+  <si>
+    <t>Exports</t>
+  </si>
+  <si>
+    <t>Domestic Use</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>BTU</t>
+  </si>
+  <si>
+    <t>uranium</t>
+  </si>
+  <si>
+    <t>Start Year Data</t>
+  </si>
+  <si>
     <t>Overall Approach and Assumptions</t>
   </si>
   <si>
-    <t>a region with non-zero changes in exports in response to chagnes in production,</t>
-  </si>
-  <si>
-    <t>https://saudiarabia.energypolicy.solutions</t>
-  </si>
-  <si>
-    <t>For an example of how to calculate the input data for this variable in</t>
-  </si>
-  <si>
-    <t>see this variable in the Saudi Arabia version of the Energy Policy Simulator:</t>
+    <t>Apportioning Secondary Product Changes to That Product vs. Crude Oil</t>
+  </si>
+  <si>
+    <t>see variable fuels/BFPIaE</t>
+  </si>
+  <si>
+    <t>We estimate the response to a drop in domestic use of a secondary petroleum product by observing how large</t>
+  </si>
+  <si>
+    <t>the export market for that fuel is, versus the domestic use market.  If the fuel's exports are a far larger share</t>
+  </si>
+  <si>
+    <t>of the total outflows (exports + use) than use is, we assume the export market for that fuel can more easily</t>
+  </si>
+  <si>
+    <t>absorb the drop in domestic production.  Where a fuel is more commonly produced for domestic use (where</t>
+  </si>
+  <si>
+    <t>use has a larger share than exports of the total outflows), we assume less of that fuel will be produced, and</t>
+  </si>
+  <si>
+    <t>more crude will be exported instead.</t>
+  </si>
+  <si>
+    <t>Reasoning</t>
+  </si>
+  <si>
+    <t>The following example may help you set this variable wisely:</t>
+  </si>
+  <si>
+    <t>Example 1: Saudi Arabia</t>
+  </si>
+  <si>
+    <t>United States Settings</t>
+  </si>
+  <si>
+    <t>Based on consultation with oil market experts at Rapidian Energy and Wood Mackenzie,</t>
+  </si>
+  <si>
+    <t>in a high electrification scenario), and the difference would be made up by increased exports,</t>
+  </si>
+  <si>
+    <t>similar to the Saudi Arabia example above.</t>
+  </si>
+  <si>
+    <t>day exports / present day production), which should roughly express how important the export market</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> for that fuel for U.S. producers.</t>
+  </si>
+  <si>
+    <t>we believe U.S. oil production would be relatively unaffected by a drop in U.S. demand (for instance,</t>
+  </si>
+  <si>
+    <t>For fuels other than crude oil and petroleum products, we use settings calculated as (present</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000E+00"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -314,7 +377,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -335,7 +398,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -353,7 +434,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -380,13 +461,52 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -660,15 +780,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H75"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -686,7 +806,7 @@
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="26" t="s">
         <v>80</v>
       </c>
     </row>
@@ -725,352 +845,759 @@
         <v>7</v>
       </c>
     </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B12" s="26" t="s">
+        <v>81</v>
+      </c>
+    </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="B13" s="27" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>21</v>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="B47" s="33"/>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>29</v>
-      </c>
-      <c r="C48" s="18"/>
-      <c r="D48" s="18"/>
-      <c r="E48" s="18"/>
-      <c r="F48" s="18"/>
-      <c r="G48" s="18"/>
-      <c r="H48" s="18"/>
+        <v>93</v>
+      </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>30</v>
-      </c>
-      <c r="C49" s="18"/>
-      <c r="D49" s="18"/>
-      <c r="E49" s="18"/>
-      <c r="F49" s="18"/>
-      <c r="G49" s="18"/>
-      <c r="H49" s="18"/>
+        <v>98</v>
+      </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>31</v>
-      </c>
-      <c r="C50" s="18"/>
-      <c r="D50" s="18"/>
-      <c r="E50" s="18"/>
-      <c r="F50" s="18"/>
-      <c r="G50" s="18"/>
-      <c r="H50" s="18"/>
+        <v>94</v>
+      </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>32</v>
-      </c>
-      <c r="C51" s="18"/>
-      <c r="D51" s="18"/>
-      <c r="E51" s="18"/>
-      <c r="F51" s="18"/>
-      <c r="G51" s="18"/>
-      <c r="H51" s="18"/>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C52" s="18"/>
-      <c r="D52" s="18"/>
-      <c r="E52" s="18"/>
-      <c r="F52" s="18"/>
-      <c r="G52" s="18"/>
-      <c r="H52" s="18"/>
+        <v>95</v>
+      </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="B53" s="13"/>
-      <c r="C53" s="18"/>
-      <c r="D53" s="18"/>
-      <c r="E53" s="18"/>
-      <c r="F53" s="18"/>
-      <c r="G53" s="18"/>
-      <c r="H53" s="18"/>
+      <c r="A53" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>64</v>
-      </c>
-      <c r="C54" s="18"/>
-      <c r="D54" s="18"/>
-      <c r="E54" s="18"/>
-      <c r="F54" s="18"/>
-      <c r="G54" s="18"/>
-      <c r="H54" s="18"/>
+        <v>96</v>
+      </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>65</v>
-      </c>
-      <c r="C55" s="18"/>
-      <c r="D55" s="18"/>
-      <c r="E55" s="18"/>
-      <c r="F55" s="18"/>
-      <c r="G55" s="18"/>
-      <c r="H55" s="18"/>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>66</v>
-      </c>
-      <c r="C56" s="18"/>
-      <c r="D56" s="18"/>
-      <c r="E56" s="18"/>
-      <c r="F56" s="18"/>
-      <c r="G56" s="18"/>
-      <c r="H56" s="18"/>
+        <v>97</v>
+      </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>67</v>
-      </c>
+      <c r="A57" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B57" s="15"/>
+      <c r="C57" s="15"/>
+      <c r="D57" s="15"/>
+      <c r="E57" s="15"/>
+      <c r="F57" s="15"/>
+      <c r="G57" s="15"/>
+      <c r="H57" s="15"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>69</v>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="B72" s="16"/>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="B73" s="16"/>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="B74" s="16"/>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="B75" s="16"/>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>62</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B7" r:id="rId1"/>
-    <hyperlink ref="B8" r:id="rId2"/>
-    <hyperlink ref="B9" r:id="rId3"/>
-    <hyperlink ref="B10" r:id="rId4"/>
-    <hyperlink ref="A75" r:id="rId5"/>
+    <hyperlink ref="B7" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B8" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B9" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B10" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:H24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="44.140625" customWidth="1"/>
+    <col min="2" max="5" width="15.42578125" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="100.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="17"/>
+      <c r="H2" s="29" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="F3" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="H3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="22"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="23"/>
+      <c r="H4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="24">
+        <v>1.2994850819999496E+16</v>
+      </c>
+      <c r="C5" s="24">
+        <v>121838241144116.98</v>
+      </c>
+      <c r="D5" s="24">
+        <v>1908500328228990.3</v>
+      </c>
+      <c r="E5" s="22">
+        <f t="shared" ref="E5:E24" si="0">B5+C5-D5</f>
+        <v>1.1208188732914622E+16</v>
+      </c>
+      <c r="F5" t="s">
+        <v>77</v>
+      </c>
+      <c r="G5" s="30"/>
+      <c r="H5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="24">
+        <v>3.3449389999999996E+16</v>
+      </c>
+      <c r="C6" s="24">
+        <v>2724850000000000</v>
+      </c>
+      <c r="D6" s="24">
+        <v>5184905000000000</v>
+      </c>
+      <c r="E6" s="22">
+        <f t="shared" si="0"/>
+        <v>3.0989335E+16</v>
+      </c>
+      <c r="F6" t="s">
+        <v>77</v>
+      </c>
+      <c r="G6" s="30"/>
+      <c r="H6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B7" s="24">
+        <v>534894468127151.31</v>
+      </c>
+      <c r="C7" s="24">
+        <v>7200000000000000</v>
+      </c>
+      <c r="D7" s="24">
+        <v>0</v>
+      </c>
+      <c r="E7" s="22">
+        <f t="shared" si="0"/>
+        <v>7734894468127151</v>
+      </c>
+      <c r="F7" t="s">
+        <v>77</v>
+      </c>
+      <c r="G7" s="30"/>
+      <c r="H7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="25"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="30"/>
+      <c r="H8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="25"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="30"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="25"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="30"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="24">
+        <v>127054236057268.86</v>
+      </c>
+      <c r="C11" s="24">
+        <v>3835846580378.2954</v>
+      </c>
+      <c r="D11" s="24">
+        <v>86443847182000</v>
+      </c>
+      <c r="E11" s="22">
+        <f t="shared" si="0"/>
+        <v>44446235455647.156</v>
+      </c>
+      <c r="F11" t="s">
+        <v>77</v>
+      </c>
+      <c r="G11" s="30"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="24">
+        <v>2.345837516236748E+16</v>
+      </c>
+      <c r="C12" s="24">
+        <v>65450425688886.055</v>
+      </c>
+      <c r="D12" s="24">
+        <v>1712687718894354.5</v>
+      </c>
+      <c r="E12" s="22">
+        <f t="shared" si="0"/>
+        <v>2.1811137869162012E+16</v>
+      </c>
+      <c r="F12" t="s">
+        <v>77</v>
+      </c>
+      <c r="G12" s="30"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="24">
+        <v>1.3635229972917368E+16</v>
+      </c>
+      <c r="C13" s="24">
+        <v>351737454255556.31</v>
+      </c>
+      <c r="D13" s="24">
+        <v>3637018944597630</v>
+      </c>
+      <c r="E13" s="22">
+        <f t="shared" si="0"/>
+        <v>1.0349948482575294E+16</v>
+      </c>
+      <c r="F13" t="s">
+        <v>77</v>
+      </c>
+      <c r="G13" s="30"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" s="24">
+        <v>1561489169872463.5</v>
+      </c>
+      <c r="C14" s="24">
+        <v>8008300000911.835</v>
+      </c>
+      <c r="D14" s="24">
+        <v>163819887068608</v>
+      </c>
+      <c r="E14" s="22">
+        <f t="shared" si="0"/>
+        <v>1405677582804767.3</v>
+      </c>
+      <c r="F14" t="s">
+        <v>77</v>
+      </c>
+      <c r="G14" s="30"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="24">
+        <v>209619113794859.22</v>
+      </c>
+      <c r="C15" s="24">
+        <v>81719279513151.391</v>
+      </c>
+      <c r="D15" s="24">
+        <v>14787150681592.84</v>
+      </c>
+      <c r="E15" s="22">
+        <f t="shared" si="0"/>
+        <v>276551242626417.78</v>
+      </c>
+      <c r="F15" t="s">
+        <v>77</v>
+      </c>
+      <c r="G15" s="30"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" s="24">
+        <v>4515477159886859</v>
+      </c>
+      <c r="C16" s="24">
+        <v>371817123993646.19</v>
+      </c>
+      <c r="D16" s="24">
+        <v>487532159271959.88</v>
+      </c>
+      <c r="E16" s="22">
+        <f t="shared" si="0"/>
+        <v>4399762124608545</v>
+      </c>
+      <c r="F16" t="s">
+        <v>77</v>
+      </c>
+      <c r="G16" s="30"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" s="25"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="30"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" s="25"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="30"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" s="24">
+        <v>859050369312946.75</v>
+      </c>
+      <c r="C19" s="24">
+        <v>0</v>
+      </c>
+      <c r="D19" s="24">
+        <v>0</v>
+      </c>
+      <c r="E19" s="22">
+        <f t="shared" si="0"/>
+        <v>859050369312946.75</v>
+      </c>
+      <c r="F19" t="s">
+        <v>77</v>
+      </c>
+      <c r="G19" s="30"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" s="24">
+        <v>2.4934676413517276E+16</v>
+      </c>
+      <c r="C20" s="24">
+        <v>1.4838296942851536E+16</v>
+      </c>
+      <c r="D20" s="24">
+        <v>2994708229987662</v>
+      </c>
+      <c r="E20" s="22">
+        <f t="shared" si="0"/>
+        <v>3.6778265126381152E+16</v>
+      </c>
+      <c r="F20" t="s">
+        <v>77</v>
+      </c>
+      <c r="G20" s="30"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" s="24">
+        <v>1250687800589910.5</v>
+      </c>
+      <c r="C21" s="24">
+        <v>476589424280788.31</v>
+      </c>
+      <c r="D21" s="24">
+        <v>873930050846522.25</v>
+      </c>
+      <c r="E21" s="22">
+        <f t="shared" si="0"/>
+        <v>853347174024176.5</v>
+      </c>
+      <c r="F21" t="s">
+        <v>77</v>
+      </c>
+      <c r="G21" s="30"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="B22" s="24">
+        <v>4084904971604980.5</v>
+      </c>
+      <c r="C22" s="24">
+        <v>243930593817797.94</v>
+      </c>
+      <c r="D22" s="24">
+        <v>1827886456100663</v>
+      </c>
+      <c r="E22" s="22">
+        <f t="shared" si="0"/>
+        <v>2500949109322115.5</v>
+      </c>
+      <c r="F22" t="s">
+        <v>77</v>
+      </c>
+      <c r="G22" s="30"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B23" s="24">
+        <v>1730154785433083.3</v>
+      </c>
+      <c r="C23" s="24">
+        <v>0</v>
+      </c>
+      <c r="D23" s="24">
+        <v>0</v>
+      </c>
+      <c r="E23" s="22">
+        <f t="shared" si="0"/>
+        <v>1730154785433083.3</v>
+      </c>
+      <c r="F23" t="s">
+        <v>77</v>
+      </c>
+      <c r="G23" s="30"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24" s="24">
+        <v>8746500000000000</v>
+      </c>
+      <c r="C24" s="24">
+        <v>0</v>
+      </c>
+      <c r="D24" s="24">
+        <v>0</v>
+      </c>
+      <c r="E24" s="22">
+        <f t="shared" si="0"/>
+        <v>8746500000000000</v>
+      </c>
+      <c r="F24" t="s">
+        <v>77</v>
+      </c>
+      <c r="G24" s="30"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
@@ -1091,75 +1618,75 @@
   <sheetData>
     <row r="1" spans="1:22" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="B1" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="L1" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="M1" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="N1" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="O1" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="P1" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="Q1" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="R1" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="S1" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="T1" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="U1" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="V1" s="10" t="s">
         <v>52</v>
-      </c>
-      <c r="M1" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="N1" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="O1" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="P1" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q1" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="R1" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="S1" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="T1" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="U1" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="V1" s="10" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="B2" s="11">
         <v>0</v>
@@ -1227,13 +1754,14 @@
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B3" s="11">
         <v>0</v>
       </c>
-      <c r="C3" s="8">
-        <v>0</v>
+      <c r="C3" s="31">
+        <f>'Data from BFPIaE'!D5/'Data from BFPIaE'!B5</f>
+        <v>0.14686588977933832</v>
       </c>
       <c r="D3" s="8">
         <v>0</v>
@@ -1295,7 +1823,7 @@
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="B4" s="11">
         <v>0</v>
@@ -1303,8 +1831,9 @@
       <c r="C4" s="8">
         <v>0</v>
       </c>
-      <c r="D4" s="8">
-        <v>0</v>
+      <c r="D4" s="31">
+        <f>'Data from BFPIaE'!D6/'Data from BFPIaE'!B6</f>
+        <v>0.15500746052469119</v>
       </c>
       <c r="E4" s="8">
         <v>0</v>
@@ -1363,7 +1892,7 @@
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="B5" s="11">
         <v>0</v>
@@ -1374,7 +1903,8 @@
       <c r="D5" s="8">
         <v>0</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="31">
+        <f>'Data from BFPIaE'!D7/'Data from BFPIaE'!B7</f>
         <v>0</v>
       </c>
       <c r="F5" s="11">
@@ -1431,7 +1961,7 @@
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="B6" s="11">
         <v>0</v>
@@ -1499,7 +2029,7 @@
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="B7" s="11">
         <v>0</v>
@@ -1567,7 +2097,7 @@
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="B8" s="11">
         <v>0</v>
@@ -1635,7 +2165,7 @@
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="B9" s="11">
         <v>0</v>
@@ -1658,8 +2188,9 @@
       <c r="H9" s="11">
         <v>0</v>
       </c>
-      <c r="I9" s="8">
-        <v>0</v>
+      <c r="I9" s="31">
+        <f>'Data from BFPIaE'!D11/'Data from BFPIaE'!B11</f>
+        <v>0.68036965837987495</v>
       </c>
       <c r="J9" s="8">
         <v>0</v>
@@ -1703,7 +2234,7 @@
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="B10" s="11">
         <v>0</v>
@@ -1729,8 +2260,9 @@
       <c r="I10" s="8">
         <v>0</v>
       </c>
-      <c r="J10" s="8">
-        <v>0</v>
+      <c r="J10" s="12">
+        <f>'Data from BFPIaE'!D12/SUM('Data from BFPIaE'!D12:E12)</f>
+        <v>7.2806513229885905E-2</v>
       </c>
       <c r="K10" s="8">
         <v>0</v>
@@ -1753,8 +2285,9 @@
       <c r="Q10" s="8">
         <v>0</v>
       </c>
-      <c r="R10" s="8">
-        <v>0</v>
+      <c r="R10" s="13">
+        <f>1-J10</f>
+        <v>0.92719348677011415</v>
       </c>
       <c r="S10" s="8">
         <v>0</v>
@@ -1771,7 +2304,7 @@
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="B11" s="11">
         <v>0</v>
@@ -1800,8 +2333,9 @@
       <c r="J11" s="8">
         <v>0</v>
       </c>
-      <c r="K11" s="8">
-        <v>0</v>
+      <c r="K11" s="12">
+        <f>'Data from BFPIaE'!D13/SUM('Data from BFPIaE'!D13:E13)</f>
+        <v>0.26002912808189416</v>
       </c>
       <c r="L11" s="8">
         <v>0</v>
@@ -1821,8 +2355,9 @@
       <c r="Q11" s="8">
         <v>0</v>
       </c>
-      <c r="R11" s="8">
-        <v>0</v>
+      <c r="R11" s="13">
+        <f>1-K11</f>
+        <v>0.73997087191810584</v>
       </c>
       <c r="S11" s="8">
         <v>0</v>
@@ -1839,7 +2374,7 @@
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="B12" s="11">
         <v>0</v>
@@ -1871,8 +2406,9 @@
       <c r="K12" s="8">
         <v>0</v>
       </c>
-      <c r="L12" s="8">
-        <v>0</v>
+      <c r="L12" s="31">
+        <f>'Data from BFPIaE'!D14/'Data from BFPIaE'!B14</f>
+        <v>0.10491259896601664</v>
       </c>
       <c r="M12" s="8">
         <v>0</v>
@@ -1907,7 +2443,7 @@
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="B13" s="11">
         <v>0</v>
@@ -1942,8 +2478,9 @@
       <c r="L13" s="8">
         <v>0</v>
       </c>
-      <c r="M13" s="8">
-        <v>0</v>
+      <c r="M13" s="31">
+        <f>'Data from BFPIaE'!D15/'Data from BFPIaE'!B15</f>
+        <v>7.0542950086431883E-2</v>
       </c>
       <c r="N13" s="8">
         <v>0</v>
@@ -1975,7 +2512,7 @@
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="B14" s="11">
         <v>0</v>
@@ -2013,8 +2550,9 @@
       <c r="M14" s="8">
         <v>0</v>
       </c>
-      <c r="N14" s="8">
-        <v>0</v>
+      <c r="N14" s="12">
+        <f>'Data from BFPIaE'!D16/SUM('Data from BFPIaE'!D16:E16)</f>
+        <v>9.9755024140854479E-2</v>
       </c>
       <c r="O14" s="11">
         <v>0</v>
@@ -2025,8 +2563,9 @@
       <c r="Q14" s="8">
         <v>0</v>
       </c>
-      <c r="R14" s="8">
-        <v>0</v>
+      <c r="R14" s="13">
+        <f>1-N14</f>
+        <v>0.90024497585914554</v>
       </c>
       <c r="S14" s="8">
         <v>0</v>
@@ -2043,7 +2582,7 @@
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="B15" s="11">
         <v>0</v>
@@ -2111,7 +2650,7 @@
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="B16" s="11">
         <v>0</v>
@@ -2179,7 +2718,7 @@
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="B17" s="11">
         <v>0</v>
@@ -2226,7 +2765,8 @@
       <c r="P17" s="11">
         <v>0</v>
       </c>
-      <c r="Q17" s="8">
+      <c r="Q17" s="31">
+        <f>'Data from BFPIaE'!D19/'Data from BFPIaE'!B19</f>
         <v>0</v>
       </c>
       <c r="R17" s="8">
@@ -2247,7 +2787,7 @@
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="B18" s="11">
         <v>0</v>
@@ -2297,8 +2837,8 @@
       <c r="Q18" s="8">
         <v>0</v>
       </c>
-      <c r="R18" s="8">
-        <v>0</v>
+      <c r="R18" s="12">
+        <v>1</v>
       </c>
       <c r="S18" s="8">
         <v>0</v>
@@ -2315,7 +2855,7 @@
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="B19" s="11">
         <v>0</v>
@@ -2365,11 +2905,13 @@
       <c r="Q19" s="8">
         <v>0</v>
       </c>
-      <c r="R19" s="8">
-        <v>0</v>
-      </c>
-      <c r="S19" s="8">
-        <v>0</v>
+      <c r="R19" s="13">
+        <f>1-S19</f>
+        <v>0.49404181432894001</v>
+      </c>
+      <c r="S19" s="12">
+        <f>'Data from BFPIaE'!D21/SUM('Data from BFPIaE'!D21:E21)</f>
+        <v>0.50595818567105999</v>
       </c>
       <c r="T19" s="8">
         <v>0</v>
@@ -2383,7 +2925,7 @@
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="B20" s="11">
         <v>0</v>
@@ -2433,14 +2975,16 @@
       <c r="Q20" s="8">
         <v>0</v>
       </c>
-      <c r="R20" s="8">
-        <v>0</v>
+      <c r="R20" s="13">
+        <f>1-T20</f>
+        <v>0.57774176716224113</v>
       </c>
       <c r="S20" s="8">
         <v>0</v>
       </c>
-      <c r="T20" s="8">
-        <v>0</v>
+      <c r="T20" s="12">
+        <f>'Data from BFPIaE'!D22/SUM('Data from BFPIaE'!D22:E22)</f>
+        <v>0.42225823283775882</v>
       </c>
       <c r="U20" s="8">
         <v>0</v>
@@ -2451,7 +2995,7 @@
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="B21" s="11">
         <v>0</v>
@@ -2510,7 +3054,8 @@
       <c r="T21" s="8">
         <v>0</v>
       </c>
-      <c r="U21" s="8">
+      <c r="U21" s="31">
+        <f>'Data from BFPIaE'!D23/'Data from BFPIaE'!B23</f>
         <v>0</v>
       </c>
       <c r="V21" s="8">
@@ -2519,7 +3064,7 @@
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="B22" s="11">
         <v>0</v>
@@ -2581,7 +3126,8 @@
       <c r="U22" s="8">
         <v>0</v>
       </c>
-      <c r="V22" s="8">
+      <c r="V22" s="31">
+        <f>'Data from BFPIaE'!D24/'Data from BFPIaE'!B24</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated with new bfpiae
</commit_message>
<xml_diff>
--- a/InputData/fuels/PoFDCtAE/Perc of Fuel Demand Changes that Affect Exports.xlsx
+++ b/InputData/fuels/PoFDCtAE/Perc of Fuel Demand Changes that Affect Exports.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeff-nonadmin\Dropbox (Energy InNovation)\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\United States\US_EPS\InputData\fuels\PoFDCtAE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{190E0567-D228-475F-AE92-CB99F12E58B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8719F1CD-7F12-4E84-8193-D1202AC966B3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2055" yWindow="1065" windowWidth="23535" windowHeight="16185" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -790,7 +790,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1129,7 +1129,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1199,17 +1201,16 @@
         <v>33</v>
       </c>
       <c r="B5" s="24">
-        <v>1.2994850819999496E+16</v>
+        <v>1.372785698375E+16</v>
       </c>
       <c r="C5" s="24">
-        <v>121838241144116.98</v>
+        <v>116791410000000</v>
       </c>
       <c r="D5" s="24">
-        <v>1908500328228990.3</v>
+        <v>1888127795000000</v>
       </c>
       <c r="E5" s="22">
-        <f t="shared" ref="E5:E24" si="0">B5+C5-D5</f>
-        <v>1.1208188732914622E+16</v>
+        <v>1.195652059875E+16</v>
       </c>
       <c r="F5" t="s">
         <v>77</v>
@@ -1224,17 +1225,16 @@
         <v>34</v>
       </c>
       <c r="B6" s="24">
-        <v>3.3449389999999996E+16</v>
+        <v>3.5698853E+16</v>
       </c>
       <c r="C6" s="24">
-        <v>2724850000000000</v>
+        <v>2791070000000000</v>
       </c>
       <c r="D6" s="24">
-        <v>5184905000000000</v>
+        <v>4483330999999999.5</v>
       </c>
       <c r="E6" s="22">
-        <f t="shared" si="0"/>
-        <v>3.0989335E+16</v>
+        <v>3.4006591999999996E+16</v>
       </c>
       <c r="F6" t="s">
         <v>77</v>
@@ -1249,7 +1249,7 @@
         <v>78</v>
       </c>
       <c r="B7" s="24">
-        <v>534894468127151.31</v>
+        <v>540000000000000</v>
       </c>
       <c r="C7" s="24">
         <v>7200000000000000</v>
@@ -1258,8 +1258,7 @@
         <v>0</v>
       </c>
       <c r="E7" s="22">
-        <f t="shared" si="0"/>
-        <v>7734894468127151</v>
+        <v>7740000000000000</v>
       </c>
       <c r="F7" t="s">
         <v>77</v>
@@ -1310,7 +1309,7 @@
         <v>39</v>
       </c>
       <c r="B11" s="24">
-        <v>127054236057268.86</v>
+        <v>123408653368000</v>
       </c>
       <c r="C11" s="24">
         <v>3835846580378.2954</v>
@@ -1319,8 +1318,7 @@
         <v>86443847182000</v>
       </c>
       <c r="E11" s="22">
-        <f t="shared" si="0"/>
-        <v>44446235455647.156</v>
+        <v>40800652766378.289</v>
       </c>
       <c r="F11" t="s">
         <v>77</v>
@@ -1332,17 +1330,16 @@
         <v>40</v>
       </c>
       <c r="B12" s="24">
-        <v>2.345837516236748E+16</v>
+        <v>1.8365288407359E+16</v>
       </c>
       <c r="C12" s="24">
-        <v>65450425688886.055</v>
+        <v>59545742184000</v>
       </c>
       <c r="D12" s="24">
-        <v>1712687718894354.5</v>
+        <v>1381937220783000</v>
       </c>
       <c r="E12" s="22">
-        <f t="shared" si="0"/>
-        <v>2.1811137869162012E+16</v>
+        <v>1.704289692876E+16</v>
       </c>
       <c r="F12" t="s">
         <v>77</v>
@@ -1354,17 +1351,16 @@
         <v>41</v>
       </c>
       <c r="B13" s="24">
-        <v>1.3635229972917368E+16</v>
+        <v>1.0682345175E+16</v>
       </c>
       <c r="C13" s="24">
-        <v>351737454255556.31</v>
+        <v>320229375000000</v>
       </c>
       <c r="D13" s="24">
-        <v>3637018944597630</v>
+        <v>2936702875000000</v>
       </c>
       <c r="E13" s="22">
-        <f t="shared" si="0"/>
-        <v>1.0349948482575294E+16</v>
+        <v>8065871675000000</v>
       </c>
       <c r="F13" t="s">
         <v>77</v>
@@ -1376,17 +1372,16 @@
         <v>42</v>
       </c>
       <c r="B14" s="24">
-        <v>1561489169872463.5</v>
+        <v>1515620096655000</v>
       </c>
       <c r="C14" s="24">
-        <v>8008300000911.835</v>
+        <v>7285809312000</v>
       </c>
       <c r="D14" s="24">
-        <v>163819887068608</v>
+        <v>132183114996000</v>
       </c>
       <c r="E14" s="22">
-        <f t="shared" si="0"/>
-        <v>1405677582804767.3</v>
+        <v>1390722790971000</v>
       </c>
       <c r="F14" t="s">
         <v>77</v>
@@ -1398,17 +1393,16 @@
         <v>43</v>
       </c>
       <c r="B15" s="24">
-        <v>209619113794859.22</v>
+        <v>203604487000000</v>
       </c>
       <c r="C15" s="24">
-        <v>81719279513151.391</v>
+        <v>74398997000000</v>
       </c>
       <c r="D15" s="24">
-        <v>14787150681592.84</v>
+        <v>11939852000000</v>
       </c>
       <c r="E15" s="22">
-        <f t="shared" si="0"/>
-        <v>276551242626417.78</v>
+        <v>266063632000000</v>
       </c>
       <c r="F15" t="s">
         <v>77</v>
@@ -1420,17 +1414,16 @@
         <v>44</v>
       </c>
       <c r="B16" s="24">
-        <v>4515477159886859</v>
+        <v>3537592380000000</v>
       </c>
       <c r="C16" s="24">
-        <v>371817123993646.19</v>
+        <v>338510340000000</v>
       </c>
       <c r="D16" s="24">
-        <v>487532159271959.88</v>
+        <v>393656760000000</v>
       </c>
       <c r="E16" s="22">
-        <f t="shared" si="0"/>
-        <v>4399762124608545</v>
+        <v>3482445960000000</v>
       </c>
       <c r="F16" t="s">
         <v>77</v>
@@ -1464,7 +1457,7 @@
         <v>47</v>
       </c>
       <c r="B19" s="24">
-        <v>859050369312946.75</v>
+        <v>906213062527442.13</v>
       </c>
       <c r="C19" s="24">
         <v>0</v>
@@ -1473,8 +1466,7 @@
         <v>0</v>
       </c>
       <c r="E19" s="22">
-        <f t="shared" si="0"/>
-        <v>859050369312946.75</v>
+        <v>906213062527442.13</v>
       </c>
       <c r="F19" t="s">
         <v>77</v>
@@ -1486,17 +1478,16 @@
         <v>48</v>
       </c>
       <c r="B20" s="24">
-        <v>2.4934676413517276E+16</v>
+        <v>1.9460537227008E+16</v>
       </c>
       <c r="C20" s="24">
-        <v>1.4838296942851536E+16</v>
+        <v>1.658307810686E+16</v>
       </c>
       <c r="D20" s="24">
-        <v>2994708229987662</v>
+        <v>2408884127644000</v>
       </c>
       <c r="E20" s="22">
-        <f t="shared" si="0"/>
-        <v>3.6778265126381152E+16</v>
+        <v>3.3634731206224E+16</v>
       </c>
       <c r="F20" t="s">
         <v>77</v>
@@ -1508,17 +1499,16 @@
         <v>49</v>
       </c>
       <c r="B21" s="24">
-        <v>1250687800589910.5</v>
+        <v>979835237000000</v>
       </c>
       <c r="C21" s="24">
-        <v>476589424280788.31</v>
+        <v>433897305000000</v>
       </c>
       <c r="D21" s="24">
-        <v>873930050846522.25</v>
+        <v>705652880000000</v>
       </c>
       <c r="E21" s="22">
-        <f t="shared" si="0"/>
-        <v>853347174024176.5</v>
+        <v>708079662000000</v>
       </c>
       <c r="F21" t="s">
         <v>77</v>
@@ -1530,17 +1520,16 @@
         <v>50</v>
       </c>
       <c r="B22" s="24">
-        <v>4084904971604980.5</v>
+        <v>3148621106400000</v>
       </c>
       <c r="C22" s="24">
-        <v>243930593817797.94</v>
+        <v>222079680900000</v>
       </c>
       <c r="D22" s="24">
-        <v>1827886456100663</v>
+        <v>1475922862260000</v>
       </c>
       <c r="E22" s="22">
-        <f t="shared" si="0"/>
-        <v>2500949109322115.5</v>
+        <v>1894777925040000</v>
       </c>
       <c r="F22" t="s">
         <v>77</v>
@@ -1552,7 +1541,7 @@
         <v>51</v>
       </c>
       <c r="B23" s="24">
-        <v>1730154785433083.3</v>
+        <v>3564295858911020.5</v>
       </c>
       <c r="C23" s="24">
         <v>0</v>
@@ -1561,8 +1550,7 @@
         <v>0</v>
       </c>
       <c r="E23" s="22">
-        <f t="shared" si="0"/>
-        <v>1730154785433083.3</v>
+        <v>3564295858911020.5</v>
       </c>
       <c r="F23" t="s">
         <v>77</v>
@@ -1583,7 +1571,6 @@
         <v>0</v>
       </c>
       <c r="E24" s="22">
-        <f t="shared" si="0"/>
         <v>8746500000000000</v>
       </c>
       <c r="F24" t="s">
@@ -1603,7 +1590,7 @@
   </sheetPr>
   <dimension ref="A1:V22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -1761,7 +1748,7 @@
       </c>
       <c r="C3" s="31">
         <f>'Data from BFPIaE'!D5/'Data from BFPIaE'!B5</f>
-        <v>0.14686588977933832</v>
+        <v>0.13753987947536334</v>
       </c>
       <c r="D3" s="8">
         <v>0</v>
@@ -1833,7 +1820,7 @@
       </c>
       <c r="D4" s="31">
         <f>'Data from BFPIaE'!D6/'Data from BFPIaE'!B6</f>
-        <v>0.15500746052469119</v>
+        <v>0.12558753638387204</v>
       </c>
       <c r="E4" s="8">
         <v>0</v>
@@ -2190,7 +2177,7 @@
       </c>
       <c r="I9" s="31">
         <f>'Data from BFPIaE'!D11/'Data from BFPIaE'!B11</f>
-        <v>0.68036965837987495</v>
+        <v>0.70046828016369056</v>
       </c>
       <c r="J9" s="8">
         <v>0</v>
@@ -2262,7 +2249,7 @@
       </c>
       <c r="J10" s="12">
         <f>'Data from BFPIaE'!D12/SUM('Data from BFPIaE'!D12:E12)</f>
-        <v>7.2806513229885905E-2</v>
+        <v>7.5004052116109651E-2</v>
       </c>
       <c r="K10" s="8">
         <v>0</v>
@@ -2287,7 +2274,7 @@
       </c>
       <c r="R10" s="13">
         <f>1-J10</f>
-        <v>0.92719348677011415</v>
+        <v>0.92499594788389039</v>
       </c>
       <c r="S10" s="8">
         <v>0</v>
@@ -2335,7 +2322,7 @@
       </c>
       <c r="K11" s="12">
         <f>'Data from BFPIaE'!D13/SUM('Data from BFPIaE'!D13:E13)</f>
-        <v>0.26002912808189416</v>
+        <v>0.26691051822957201</v>
       </c>
       <c r="L11" s="8">
         <v>0</v>
@@ -2357,7 +2344,7 @@
       </c>
       <c r="R11" s="13">
         <f>1-K11</f>
-        <v>0.73997087191810584</v>
+        <v>0.73308948177042799</v>
       </c>
       <c r="S11" s="8">
         <v>0</v>
@@ -2408,7 +2395,7 @@
       </c>
       <c r="L12" s="31">
         <f>'Data from BFPIaE'!D14/'Data from BFPIaE'!B14</f>
-        <v>0.10491259896601664</v>
+        <v>8.7213883800914521E-2</v>
       </c>
       <c r="M12" s="8">
         <v>0</v>
@@ -2480,7 +2467,7 @@
       </c>
       <c r="M13" s="31">
         <f>'Data from BFPIaE'!D15/'Data from BFPIaE'!B15</f>
-        <v>7.0542950086431883E-2</v>
+        <v>5.8642381491327347E-2</v>
       </c>
       <c r="N13" s="8">
         <v>0</v>
@@ -2552,7 +2539,7 @@
       </c>
       <c r="N14" s="12">
         <f>'Data from BFPIaE'!D16/SUM('Data from BFPIaE'!D16:E16)</f>
-        <v>9.9755024140854479E-2</v>
+        <v>0.10155994008332163</v>
       </c>
       <c r="O14" s="11">
         <v>0</v>
@@ -2565,7 +2552,7 @@
       </c>
       <c r="R14" s="13">
         <f>1-N14</f>
-        <v>0.90024497585914554</v>
+        <v>0.89844005991667841</v>
       </c>
       <c r="S14" s="8">
         <v>0</v>
@@ -2907,11 +2894,11 @@
       </c>
       <c r="R19" s="13">
         <f>1-S19</f>
-        <v>0.49404181432894001</v>
+        <v>0.50085828893652218</v>
       </c>
       <c r="S19" s="12">
         <f>'Data from BFPIaE'!D21/SUM('Data from BFPIaE'!D21:E21)</f>
-        <v>0.50595818567105999</v>
+        <v>0.49914171106347782</v>
       </c>
       <c r="T19" s="8">
         <v>0</v>
@@ -2977,14 +2964,14 @@
       </c>
       <c r="R20" s="13">
         <f>1-T20</f>
-        <v>0.57774176716224113</v>
+        <v>0.56213174784871833</v>
       </c>
       <c r="S20" s="8">
         <v>0</v>
       </c>
       <c r="T20" s="12">
         <f>'Data from BFPIaE'!D22/SUM('Data from BFPIaE'!D22:E22)</f>
-        <v>0.42225823283775882</v>
+        <v>0.43786825215128167</v>
       </c>
       <c r="U20" s="8">
         <v>0</v>

</xml_diff>

<commit_message>
AEO updates to fuels/BFPIaE, fuels/BS, fuels/PoFDCtAE
</commit_message>
<xml_diff>
--- a/InputData/fuels/PoFDCtAE/Perc of Fuel Demand Changes that Affect Exports.xlsx
+++ b/InputData/fuels/PoFDCtAE/Perc of Fuel Demand Changes that Affect Exports.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\United States\US_EPS\InputData\fuels\PoFDCtAE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shelley\Dropbox (Energy Innovation)\PC (2)\Documents\GitHub_Repositories\eps-us\InputData\fuels\PoFDCtAE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8719F1CD-7F12-4E84-8193-D1202AC966B3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{864A75DB-5DCF-48DD-815D-5DA8E9B27952}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15345" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -790,19 +790,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H74"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="87.5703125" customWidth="1"/>
+    <col min="2" max="2" width="87.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -810,223 +810,223 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B5" s="2">
         <v>2018</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B7" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B8" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B9" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B10" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B12" s="26" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B13" s="27" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" s="32" t="s">
         <v>92</v>
       </c>
       <c r="B47" s="33"/>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A57" s="14" t="s">
         <v>53</v>
       </c>
@@ -1038,77 +1038,77 @@
       <c r="G57" s="15"/>
       <c r="H57" s="15"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>62</v>
       </c>
@@ -1130,24 +1130,24 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="44.140625" customWidth="1"/>
-    <col min="2" max="5" width="15.42578125" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="100.7109375" customWidth="1"/>
+    <col min="1" max="1" width="44.1796875" customWidth="1"/>
+    <col min="2" max="5" width="15.453125" customWidth="1"/>
+    <col min="6" max="6" width="12.81640625" customWidth="1"/>
+    <col min="7" max="7" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="100.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="14" t="s">
         <v>70</v>
       </c>
@@ -1160,7 +1160,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="18" t="s">
         <v>71</v>
       </c>
@@ -1183,7 +1183,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>32</v>
       </c>
@@ -1196,7 +1196,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
         <v>33</v>
       </c>
@@ -1220,7 +1220,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
         <v>34</v>
       </c>
@@ -1244,7 +1244,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
         <v>78</v>
       </c>
@@ -1268,7 +1268,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>36</v>
       </c>
@@ -1282,7 +1282,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>37</v>
       </c>
@@ -1293,7 +1293,7 @@
       <c r="F9" s="23"/>
       <c r="G9" s="30"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
         <v>38</v>
       </c>
@@ -1304,28 +1304,28 @@
       <c r="F10" s="23"/>
       <c r="G10" s="30"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="6" t="s">
         <v>39</v>
       </c>
       <c r="B11" s="24">
-        <v>123408653368000</v>
+        <v>166043036334000</v>
       </c>
       <c r="C11" s="24">
-        <v>3835846580378.2954</v>
+        <v>5522103312930.1787</v>
       </c>
       <c r="D11" s="24">
-        <v>86443847182000</v>
+        <v>124444981024000</v>
       </c>
       <c r="E11" s="22">
-        <v>40800652766378.289</v>
+        <v>47120158622930.172</v>
       </c>
       <c r="F11" t="s">
         <v>77</v>
       </c>
       <c r="G11" s="30"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="28" t="s">
         <v>40</v>
       </c>
@@ -1346,7 +1346,7 @@
       </c>
       <c r="G12" s="30"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="28" t="s">
         <v>41</v>
       </c>
@@ -1367,7 +1367,7 @@
       </c>
       <c r="G13" s="30"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="6" t="s">
         <v>42</v>
       </c>
@@ -1388,7 +1388,7 @@
       </c>
       <c r="G14" s="30"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="6" t="s">
         <v>43</v>
       </c>
@@ -1409,7 +1409,7 @@
       </c>
       <c r="G15" s="30"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="28" t="s">
         <v>44</v>
       </c>
@@ -1430,7 +1430,7 @@
       </c>
       <c r="G16" s="30"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="7" t="s">
         <v>45</v>
       </c>
@@ -1441,7 +1441,7 @@
       <c r="F17" s="23"/>
       <c r="G17" s="30"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="7" t="s">
         <v>46</v>
       </c>
@@ -1452,7 +1452,7 @@
       <c r="F18" s="23"/>
       <c r="G18" s="30"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="6" t="s">
         <v>47</v>
       </c>
@@ -1473,7 +1473,7 @@
       </c>
       <c r="G19" s="30"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="6" t="s">
         <v>48</v>
       </c>
@@ -1494,7 +1494,7 @@
       </c>
       <c r="G20" s="30"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="28" t="s">
         <v>49</v>
       </c>
@@ -1515,7 +1515,7 @@
       </c>
       <c r="G21" s="30"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="28" t="s">
         <v>50</v>
       </c>
@@ -1536,7 +1536,7 @@
       </c>
       <c r="G22" s="30"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" s="6" t="s">
         <v>51</v>
       </c>
@@ -1557,7 +1557,7 @@
       </c>
       <c r="G23" s="30"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="6" t="s">
         <v>52</v>
       </c>
@@ -1590,20 +1590,20 @@
   </sheetPr>
   <dimension ref="A1:V22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="36.7109375" customWidth="1"/>
-    <col min="2" max="22" width="16.5703125" style="8" customWidth="1"/>
+    <col min="1" max="1" width="36.7265625" customWidth="1"/>
+    <col min="2" max="22" width="16.54296875" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>69</v>
       </c>
@@ -1671,7 +1671,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>32</v>
       </c>
@@ -1739,7 +1739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>33</v>
       </c>
@@ -1808,7 +1808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
         <v>34</v>
       </c>
@@ -1877,7 +1877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
         <v>35</v>
       </c>
@@ -1946,7 +1946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
         <v>36</v>
       </c>
@@ -2014,7 +2014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
         <v>37</v>
       </c>
@@ -2082,7 +2082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>38</v>
       </c>
@@ -2150,7 +2150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="s">
         <v>39</v>
       </c>
@@ -2177,7 +2177,7 @@
       </c>
       <c r="I9" s="31">
         <f>'Data from BFPIaE'!D11/'Data from BFPIaE'!B11</f>
-        <v>0.70046828016369056</v>
+        <v>0.74947425541939383</v>
       </c>
       <c r="J9" s="8">
         <v>0</v>
@@ -2219,7 +2219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A10" s="6" t="s">
         <v>40</v>
       </c>
@@ -2289,7 +2289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A11" s="6" t="s">
         <v>41</v>
       </c>
@@ -2359,7 +2359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A12" s="6" t="s">
         <v>42</v>
       </c>
@@ -2428,7 +2428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A13" s="6" t="s">
         <v>43</v>
       </c>
@@ -2497,7 +2497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A14" s="6" t="s">
         <v>44</v>
       </c>
@@ -2567,7 +2567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A15" s="7" t="s">
         <v>45</v>
       </c>
@@ -2635,7 +2635,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A16" s="7" t="s">
         <v>46</v>
       </c>
@@ -2703,7 +2703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A17" s="6" t="s">
         <v>47</v>
       </c>
@@ -2772,7 +2772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A18" s="6" t="s">
         <v>48</v>
       </c>
@@ -2840,7 +2840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A19" s="6" t="s">
         <v>49</v>
       </c>
@@ -2910,7 +2910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A20" s="6" t="s">
         <v>50</v>
       </c>
@@ -2980,7 +2980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A21" s="6" t="s">
         <v>51</v>
       </c>
@@ -3049,7 +3049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A22" s="6" t="s">
         <v>52</v>
       </c>

</xml_diff>

<commit_message>
Correction for AEO 2023 BFPIaE, IMFPbFT, and PoFDCtAE updates
</commit_message>
<xml_diff>
--- a/InputData/fuels/PoFDCtAE/Perc of Fuel Demand Changes that Affect Exports.xlsx
+++ b/InputData/fuels/PoFDCtAE/Perc of Fuel Demand Changes that Affect Exports.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mary Francis Swint\Vensim\eps-us\InputData\fuels\PoFDCtAE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3080F3D-E11E-4DBB-BBED-152C18825466}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39172FEF-DF46-4438-98F5-4879A2699F7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19305" yWindow="-5760" windowWidth="19410" windowHeight="20985" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -1126,7 +1126,7 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
No IRA AEO Updates Part 4
</commit_message>
<xml_diff>
--- a/InputData/fuels/PoFDCtAE/Perc of Fuel Demand Changes that Affect Exports.xlsx
+++ b/InputData/fuels/PoFDCtAE/Perc of Fuel Demand Changes that Affect Exports.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mary Francis Swint\Vensim\eps-us\InputData\fuels\PoFDCtAE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39172FEF-DF46-4438-98F5-4879A2699F7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{944C047B-153C-458A-AE04-46EA9661B408}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19305" yWindow="-5760" windowWidth="19410" windowHeight="20985" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28695" yWindow="-2835" windowWidth="14610" windowHeight="15585" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -1126,7 +1126,7 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1539,7 +1539,7 @@
         <v>52</v>
       </c>
       <c r="B24" s="22">
-        <v>8746500000000000</v>
+        <v>1345098039215686.5</v>
       </c>
       <c r="C24" s="22">
         <v>0</v>
@@ -1548,7 +1548,7 @@
         <v>0</v>
       </c>
       <c r="E24" s="20">
-        <v>8746500000000000</v>
+        <v>1345098039215686.5</v>
       </c>
       <c r="F24" t="s">
         <v>77</v>

</xml_diff>